<commit_message>
DC team quiz alignment changed
</commit_message>
<xml_diff>
--- a/Team PPTs/N. Swetha/Terminal Sterilization Spreadsheet-N.SWETHA.xlsx
+++ b/Team PPTs/N. Swetha/Terminal Sterilization Spreadsheet-N.SWETHA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sweth\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkuma\Documents\Conference NOV 2023\Team PPTs\N. Swetha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD84F402-8E9C-4B16-B29B-6B8694630DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC4AAA2-AA34-45C4-8607-1ADF1286DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{79137C92-F9A1-479A-85FF-32393231CFD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{79137C92-F9A1-479A-85FF-32393231CFD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminal Sterilization" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -152,15 +152,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -170,6 +180,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,128 +507,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA572E8-2562-4485-A594-E7139D3DC374}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
-    <col min="8" max="10" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="11" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+  <mergeCells count="13">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>